<commit_message>
add plotting coast overview script
</commit_message>
<xml_diff>
--- a/MD_13Oct2021/ws_data/InitialEmittances_growth_rate.xlsx
+++ b/MD_13Oct2021/ws_data/InitialEmittances_growth_rate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>coast1-setting0</t>
   </si>
@@ -46,7 +46,7 @@
     <t>coast3-setting3</t>
   </si>
   <si>
-    <t>ayy, axy values for the ΔQy rms computation</t>
+    <t>ayy, axy values for the ΔQy rms computation, using [5]</t>
   </si>
   <si>
     <t>k_LOD = 0 [1/m^4]</t>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>https://github.com/natriant/exploring_SPS/blob/master/match_octupoles/job004_matching_ayyScan.py</t>
+  </si>
+  <si>
+    <t>[5]</t>
+  </si>
+  <si>
+    <t>https://github.com/natriant/CC_MD_2021/blob/master/helper_scripts/cmpt_tuneSpread_for_givenEmitandOctupoleSettings.py</t>
   </si>
 </sst>
 </file>
@@ -758,12 +764,21 @@
         <v>28</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B38"/>
     <hyperlink r:id="rId2" ref="B39"/>
     <hyperlink r:id="rId3" ref="B41"/>
+    <hyperlink r:id="rId4" ref="B42"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>